<commit_message>
changed parameter names for recovery functions for general distribution
</commit_message>
<xml_diff>
--- a/tests/models/test_network__basic/input/model_simple_network.xlsx
+++ b/tests/models/test_network__basic/input/model_simple_network.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marufr/code/testcode/tests/models/test_network__basic/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marufr/code/sira/tests/models/test_network__basic/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEB123D-BF1C-2043-96AE-F6A7A87CC2BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C693317-671A-344B-80D9-3932917B20D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28780" windowHeight="17440" tabRatio="937" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,12 +114,6 @@
     <t>minimum</t>
   </si>
   <si>
-    <t>recovery_mean</t>
-  </si>
-  <si>
-    <t>recovery_std</t>
-  </si>
-  <si>
     <t>recovery_95percentile</t>
   </si>
   <si>
@@ -457,9 +451,6 @@
     <t>recovery_function</t>
   </si>
   <si>
-    <t>Normal</t>
-  </si>
-  <si>
     <t>Output capacity measured in MW.</t>
   </si>
   <si>
@@ -677,6 +668,15 @@
   </si>
   <si>
     <t>Water Supply Commercial</t>
+  </si>
+  <si>
+    <t>recovery_param1</t>
+  </si>
+  <si>
+    <t>recovery_param2</t>
+  </si>
+  <si>
+    <t>Rayleigh</t>
   </si>
 </sst>
 </file>
@@ -2269,84 +2269,84 @@
   <sheetData>
     <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="68" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B1" s="68" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C1" s="68" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="65" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="113" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B2" s="63" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C2" s="64"/>
     </row>
     <row r="3" spans="1:3" s="65" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="62" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B3" s="63" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C3" s="64"/>
     </row>
     <row r="4" spans="1:3" s="65" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="62" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B4" s="63" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C4" s="64"/>
     </row>
     <row r="5" spans="1:3" s="65" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="62" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B5" s="94" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C5" s="64"/>
     </row>
     <row r="6" spans="1:3" s="65" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="62" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B6" s="63" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C6" s="64"/>
     </row>
     <row r="7" spans="1:3" s="65" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="62" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B7" s="63" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C7" s="64"/>
     </row>
     <row r="8" spans="1:3" s="65" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="62" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B8" s="63" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C8" s="64"/>
     </row>
     <row r="9" spans="1:3" s="65" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="62" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B9" s="63" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C9" s="64"/>
     </row>
@@ -2512,88 +2512,88 @@
   <sheetData>
     <row r="1" spans="1:3" s="89" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="88" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="88" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="88" t="s">
-        <v>140</v>
-      </c>
       <c r="C1" s="88" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="5" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="90" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B2" s="90"/>
       <c r="C2" s="90"/>
     </row>
     <row r="3" spans="1:3" s="5" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="90" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B3" s="90"/>
       <c r="C3" s="90"/>
     </row>
     <row r="4" spans="1:3" s="5" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="90" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B4" s="90"/>
       <c r="C4" s="90"/>
     </row>
     <row r="5" spans="1:3" s="5" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="90" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B5" s="90"/>
       <c r="C5" s="90"/>
     </row>
     <row r="6" spans="1:3" s="5" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="90" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B6" s="90"/>
       <c r="C6" s="90"/>
     </row>
     <row r="7" spans="1:3" s="5" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="90" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B7" s="90"/>
       <c r="C7" s="90"/>
     </row>
     <row r="8" spans="1:3" s="5" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="90" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B8" s="90"/>
       <c r="C8" s="90"/>
     </row>
     <row r="9" spans="1:3" s="5" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="90" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B9" s="90"/>
       <c r="C9" s="90"/>
     </row>
     <row r="10" spans="1:3" s="5" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="90" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B10" s="90"/>
       <c r="C10" s="90"/>
     </row>
     <row r="11" spans="1:3" s="5" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="90" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B11" s="90"/>
       <c r="C11" s="90"/>
     </row>
     <row r="12" spans="1:3" s="5" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="90" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" s="90"/>
       <c r="C12" s="90"/>
@@ -2958,126 +2958,126 @@
   <sheetData>
     <row r="1" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="60" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="58" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B2" s="57"/>
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="59" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="59" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="59" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="59" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="59" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="59" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:2" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="59" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="59" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="59" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:2" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="59" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="59" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="59" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:2" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="59" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:2" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="59" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="3:3" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3105,42 +3105,42 @@
   <sheetData>
     <row r="1" spans="1:18" s="20" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F1" s="129" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G1" s="130"/>
       <c r="H1" s="130"/>
       <c r="I1" s="129" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J1" s="130"/>
       <c r="K1" s="130"/>
       <c r="L1" s="129" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M1" s="130"/>
       <c r="N1" s="130"/>
       <c r="O1" s="129" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="P1" s="130"/>
       <c r="Q1" s="130"/>
       <c r="R1" s="32" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -3150,40 +3150,40 @@
       <c r="D2" s="22"/>
       <c r="E2" s="38"/>
       <c r="F2" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="L2" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="M2" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="N2" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="O2" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="P2" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="Q2" s="29" t="s">
         <v>88</v>
-      </c>
-      <c r="L2" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="M2" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="N2" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="O2" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="P2" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q2" s="29" t="s">
-        <v>90</v>
       </c>
       <c r="R2" s="33"/>
     </row>
@@ -3194,40 +3194,40 @@
       <c r="D3" s="23"/>
       <c r="E3" s="39"/>
       <c r="F3" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="G3" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="H3" s="23" t="s">
-        <v>93</v>
-      </c>
       <c r="I3" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="K3" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="J3" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="K3" s="23" t="s">
-        <v>93</v>
-      </c>
       <c r="L3" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="M3" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="N3" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="M3" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="N3" s="23" t="s">
-        <v>93</v>
-      </c>
       <c r="O3" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="P3" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q3" s="23" t="s">
         <v>91</v>
-      </c>
-      <c r="P3" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q3" s="23" t="s">
-        <v>93</v>
       </c>
       <c r="R3" s="34"/>
     </row>
@@ -3836,74 +3836,74 @@
   <sheetData>
     <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="68" t="s">
         <v>65</v>
-      </c>
-      <c r="B1" s="68" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="68" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="17" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="69" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="17" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="69" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>69</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="17" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="69" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>72</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="17" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="69" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C5" s="18"/>
     </row>
     <row r="6" spans="1:3" s="17" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="69" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="17" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="69" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C7" s="18"/>
     </row>
@@ -4092,33 +4092,33 @@
         <v>5</v>
       </c>
       <c r="G1" s="116" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H1" s="116" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I1" s="116" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="103" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B2" s="117" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C2" s="104" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D2" s="105">
         <v>0</v>
       </c>
       <c r="E2" s="106" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F2" s="104" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G2" s="107">
         <v>1</v>
@@ -4134,22 +4134,22 @@
     </row>
     <row r="3" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="103" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B3" s="108" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C3" s="104" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D3" s="105">
         <v>0</v>
       </c>
       <c r="E3" s="106" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F3" s="104" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G3" s="107">
         <v>1</v>
@@ -4165,22 +4165,22 @@
     </row>
     <row r="4" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="118" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B4" s="104" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C4" s="104" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D4" s="105">
         <v>0.35</v>
       </c>
       <c r="E4" s="104" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F4" s="104" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G4" s="107">
         <v>1</v>
@@ -4196,22 +4196,22 @@
     </row>
     <row r="5" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="118" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" s="104" t="s">
         <v>159</v>
       </c>
-      <c r="B5" s="104" t="s">
-        <v>162</v>
-      </c>
       <c r="C5" s="104" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D5" s="105">
         <v>0.35</v>
       </c>
       <c r="E5" s="104" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F5" s="104" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G5" s="107">
         <v>1</v>
@@ -4227,22 +4227,22 @@
     </row>
     <row r="6" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="118" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B6" s="104" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C6" s="104" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D6" s="105">
         <v>0.3</v>
       </c>
       <c r="E6" s="104" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F6" s="104" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G6" s="107">
         <v>1</v>
@@ -4331,10 +4331,10 @@
     </row>
     <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C2" s="52">
         <v>1</v>
@@ -4345,10 +4345,10 @@
     </row>
     <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C3" s="52">
         <v>1</v>
@@ -4359,10 +4359,10 @@
     </row>
     <row r="4" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C4" s="52">
         <v>1</v>
@@ -4373,10 +4373,10 @@
     </row>
     <row r="5" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C5" s="52">
         <v>1</v>
@@ -5391,7 +5391,7 @@
     </row>
     <row r="2" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="109" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B2" s="50">
         <v>1000</v>
@@ -5400,7 +5400,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="46" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -5470,10 +5470,10 @@
     </row>
     <row r="2" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="110" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B2" s="44" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C2" s="45">
         <v>500</v>
@@ -5548,10 +5548,10 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="K10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I6" sqref="I6:J9"/>
+      <selection pane="bottomRight" activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5575,7 +5575,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="76" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B1" s="77" t="s">
         <v>1</v>
@@ -5584,19 +5584,19 @@
         <v>19</v>
       </c>
       <c r="D1" s="77" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E1" s="77" t="s">
         <v>20</v>
       </c>
       <c r="F1" s="78" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G1" s="78" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H1" s="78" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I1" s="78" t="s">
         <v>21</v>
@@ -5608,25 +5608,25 @@
         <v>23</v>
       </c>
       <c r="L1" s="79" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="M1" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="N1" s="84" t="s">
         <v>108</v>
       </c>
-      <c r="N1" s="84" t="s">
-        <v>110</v>
-      </c>
       <c r="O1" s="82" t="s">
+        <v>182</v>
+      </c>
+      <c r="P1" s="82" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q1" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="82" t="s">
+      <c r="R1" s="81" t="s">
         <v>25</v>
-      </c>
-      <c r="Q1" s="80" t="s">
-        <v>26</v>
-      </c>
-      <c r="R1" s="81" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.15">
@@ -5635,16 +5635,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C2" s="120" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F2" s="72">
         <v>0.23</v>
@@ -5662,7 +5662,7 @@
         <v>1</v>
       </c>
       <c r="K2" s="74" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L2" s="74">
         <v>0.01</v>
@@ -5671,19 +5671,19 @@
         <v>0.95</v>
       </c>
       <c r="N2" s="85" t="s">
-        <v>111</v>
+        <v>184</v>
       </c>
       <c r="O2" s="99">
-        <v>1.6710292746097057</v>
+        <v>0</v>
       </c>
       <c r="P2" s="83">
-        <v>0.2</v>
+        <v>3</v>
       </c>
       <c r="Q2" s="100">
         <v>2</v>
       </c>
       <c r="R2" s="13" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.15">
@@ -5692,16 +5692,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C3" s="121" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F3" s="72">
         <v>0.38</v>
@@ -5719,7 +5719,7 @@
         <v>1</v>
       </c>
       <c r="K3" s="74" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L3" s="74">
         <v>0.05</v>
@@ -5728,13 +5728,13 @@
         <v>0.75</v>
       </c>
       <c r="N3" s="85" t="s">
-        <v>111</v>
+        <v>184</v>
       </c>
       <c r="O3" s="99">
-        <v>4.1775731865242642</v>
+        <v>1</v>
       </c>
       <c r="P3" s="83">
-        <v>0.5</v>
+        <v>7</v>
       </c>
       <c r="Q3" s="100">
         <v>5</v>
@@ -5747,16 +5747,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C4" s="121" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F4" s="72">
         <v>0.55000000000000004</v>
@@ -5774,7 +5774,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="74" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L4" s="74">
         <v>0.3</v>
@@ -5783,13 +5783,13 @@
         <v>0.3</v>
       </c>
       <c r="N4" s="85" t="s">
-        <v>111</v>
+        <v>184</v>
       </c>
       <c r="O4" s="99">
-        <v>50.130878238291174</v>
+        <v>2</v>
       </c>
       <c r="P4" s="83">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="Q4" s="100">
         <v>60</v>
@@ -5802,16 +5802,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C5" s="122" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F5" s="72">
         <v>0.8</v>
@@ -5829,7 +5829,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="74" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L5" s="74">
         <v>1</v>
@@ -5838,13 +5838,13 @@
         <v>0</v>
       </c>
       <c r="N5" s="85" t="s">
-        <v>111</v>
+        <v>184</v>
       </c>
       <c r="O5" s="99">
-        <v>125.32719559572793</v>
+        <v>5</v>
       </c>
       <c r="P5" s="83">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="Q5" s="100">
         <v>150</v>
@@ -5857,16 +5857,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="71" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C6" s="120" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F6" s="72">
         <v>0.15</v>
@@ -5884,7 +5884,7 @@
         <v>0.95</v>
       </c>
       <c r="K6" s="74" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L6" s="74">
         <v>0.01</v>
@@ -5893,19 +5893,19 @@
         <v>0.95</v>
       </c>
       <c r="N6" s="85" t="s">
-        <v>111</v>
+        <v>184</v>
       </c>
       <c r="O6" s="99">
-        <v>0.83551463730485287</v>
+        <v>0</v>
       </c>
       <c r="P6" s="83">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="Q6" s="12">
         <v>1</v>
       </c>
       <c r="R6" s="13" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.15">
@@ -5914,16 +5914,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="71" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C7" s="121" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F7" s="72">
         <v>0.7</v>
@@ -5941,7 +5941,7 @@
         <v>0.75</v>
       </c>
       <c r="K7" s="74" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L7" s="74">
         <v>0.05</v>
@@ -5950,13 +5950,13 @@
         <v>0.75</v>
       </c>
       <c r="N7" s="85" t="s">
-        <v>111</v>
+        <v>184</v>
       </c>
       <c r="O7" s="99">
-        <v>1.6710292746097057</v>
+        <v>1</v>
       </c>
       <c r="P7" s="83">
-        <v>0.2</v>
+        <v>3</v>
       </c>
       <c r="Q7" s="12">
         <v>2</v>
@@ -5969,16 +5969,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="71" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C8" s="121" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F8" s="72">
         <v>101</v>
@@ -5996,7 +5996,7 @@
         <v>0.3</v>
       </c>
       <c r="K8" s="74" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L8" s="74">
         <v>1</v>
@@ -6005,13 +6005,13 @@
         <v>0.3</v>
       </c>
       <c r="N8" s="85" t="s">
-        <v>111</v>
+        <v>184</v>
       </c>
       <c r="O8" s="99">
-        <v>83.551463730485281</v>
+        <v>2</v>
       </c>
       <c r="P8" s="83">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="Q8" s="12">
         <v>100</v>
@@ -6024,16 +6024,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="71" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C9" s="122" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F9" s="72">
         <v>101</v>
@@ -6051,7 +6051,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="74" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L9" s="74">
         <v>1</v>
@@ -6060,13 +6060,13 @@
         <v>0</v>
       </c>
       <c r="N9" s="85" t="s">
-        <v>111</v>
+        <v>184</v>
       </c>
       <c r="O9" s="99">
-        <v>125.32719559572793</v>
+        <v>2</v>
       </c>
       <c r="P9" s="83">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q9" s="12">
         <v>150</v>
@@ -6079,16 +6079,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="92" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10" s="120" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F10" s="75">
         <v>101</v>
@@ -6106,7 +6106,7 @@
         <v>1</v>
       </c>
       <c r="K10" s="74" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L10" s="74">
         <v>0</v>
@@ -6115,19 +6115,19 @@
         <v>1</v>
       </c>
       <c r="N10" s="85" t="s">
-        <v>111</v>
+        <v>184</v>
       </c>
       <c r="O10" s="99">
-        <v>0.41775731865242643</v>
+        <v>0</v>
       </c>
       <c r="P10" s="83">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="Q10" s="14">
         <v>0.5</v>
       </c>
       <c r="R10" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.15">
@@ -6136,16 +6136,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="92" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C11" s="121" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F11" s="75">
         <v>101</v>
@@ -6163,7 +6163,7 @@
         <v>1</v>
       </c>
       <c r="K11" s="74" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L11" s="74">
         <v>0</v>
@@ -6172,13 +6172,13 @@
         <v>1</v>
       </c>
       <c r="N11" s="85" t="s">
-        <v>111</v>
+        <v>184</v>
       </c>
       <c r="O11" s="99">
-        <v>0.83551463730485287</v>
+        <v>0</v>
       </c>
       <c r="P11" s="83">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="Q11" s="14">
         <v>1</v>
@@ -6191,16 +6191,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="92" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12" s="121" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F12" s="75">
         <v>101</v>
@@ -6218,7 +6218,7 @@
         <v>1</v>
       </c>
       <c r="K12" s="74" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L12" s="74">
         <v>0</v>
@@ -6227,13 +6227,13 @@
         <v>1</v>
       </c>
       <c r="N12" s="85" t="s">
-        <v>111</v>
+        <v>184</v>
       </c>
       <c r="O12" s="99">
-        <v>1.6710292746097057</v>
+        <v>0</v>
       </c>
       <c r="P12" s="83">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="Q12" s="14">
         <v>2</v>
@@ -6246,16 +6246,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="92" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C13" s="122" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F13" s="75">
         <v>101</v>
@@ -6273,7 +6273,7 @@
         <v>1</v>
       </c>
       <c r="K13" s="74" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L13" s="74">
         <v>0</v>
@@ -6282,13 +6282,13 @@
         <v>1</v>
       </c>
       <c r="N13" s="85" t="s">
-        <v>111</v>
+        <v>184</v>
       </c>
       <c r="O13" s="99">
-        <v>3.3420585492194115</v>
+        <v>0</v>
       </c>
       <c r="P13" s="83">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="Q13" s="14">
         <v>4</v>
@@ -6301,16 +6301,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="92" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C14" s="120" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F14" s="75">
         <v>101</v>
@@ -6328,7 +6328,7 @@
         <v>1</v>
       </c>
       <c r="K14" s="74" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L14" s="74">
         <v>0</v>
@@ -6337,19 +6337,19 @@
         <v>1</v>
       </c>
       <c r="N14" s="85" t="s">
-        <v>111</v>
+        <v>184</v>
       </c>
       <c r="O14" s="99">
-        <v>0.41775731865242643</v>
+        <v>0</v>
       </c>
       <c r="P14" s="83">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="Q14" s="14">
         <v>0.5</v>
       </c>
       <c r="R14" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.15">
@@ -6358,16 +6358,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="92" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C15" s="121" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F15" s="75">
         <v>101</v>
@@ -6385,7 +6385,7 @@
         <v>1</v>
       </c>
       <c r="K15" s="74" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L15" s="74">
         <v>0</v>
@@ -6394,13 +6394,13 @@
         <v>1</v>
       </c>
       <c r="N15" s="85" t="s">
-        <v>111</v>
+        <v>184</v>
       </c>
       <c r="O15" s="99">
-        <v>0.83551463730485287</v>
+        <v>0</v>
       </c>
       <c r="P15" s="83">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="Q15" s="14">
         <v>1</v>
@@ -6413,16 +6413,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="92" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C16" s="121" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F16" s="75">
         <v>101</v>
@@ -6440,7 +6440,7 @@
         <v>1</v>
       </c>
       <c r="K16" s="74" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L16" s="74">
         <v>0</v>
@@ -6449,13 +6449,13 @@
         <v>1</v>
       </c>
       <c r="N16" s="85" t="s">
-        <v>111</v>
+        <v>184</v>
       </c>
       <c r="O16" s="99">
-        <v>1.6710292746097057</v>
+        <v>0</v>
       </c>
       <c r="P16" s="83">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="Q16" s="14">
         <v>2</v>
@@ -6468,16 +6468,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="92" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C17" s="122" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F17" s="75">
         <v>101</v>
@@ -6495,7 +6495,7 @@
         <v>1</v>
       </c>
       <c r="K17" s="74" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L17" s="74">
         <v>0</v>
@@ -6504,13 +6504,13 @@
         <v>1</v>
       </c>
       <c r="N17" s="85" t="s">
-        <v>111</v>
+        <v>184</v>
       </c>
       <c r="O17" s="99">
-        <v>3.3420585492194115</v>
+        <v>0</v>
       </c>
       <c r="P17" s="83">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="Q17" s="14">
         <v>4</v>
@@ -6523,16 +6523,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="92" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C18" s="120" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F18" s="75">
         <v>101</v>
@@ -6550,7 +6550,7 @@
         <v>1</v>
       </c>
       <c r="K18" s="74" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L18" s="74">
         <v>0</v>
@@ -6559,19 +6559,19 @@
         <v>1</v>
       </c>
       <c r="N18" s="85" t="s">
-        <v>111</v>
+        <v>184</v>
       </c>
       <c r="O18" s="99">
-        <v>0.41775731865242643</v>
+        <v>0</v>
       </c>
       <c r="P18" s="83">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="Q18" s="14">
         <v>0.5</v>
       </c>
       <c r="R18" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.15">
@@ -6580,16 +6580,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="92" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C19" s="121" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F19" s="75">
         <v>101</v>
@@ -6607,7 +6607,7 @@
         <v>1</v>
       </c>
       <c r="K19" s="74" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L19" s="74">
         <v>0</v>
@@ -6616,19 +6616,19 @@
         <v>1</v>
       </c>
       <c r="N19" s="85" t="s">
-        <v>111</v>
+        <v>184</v>
       </c>
       <c r="O19" s="99">
-        <v>0.83551463730485287</v>
+        <v>0</v>
       </c>
       <c r="P19" s="83">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="Q19" s="14">
         <v>1</v>
       </c>
       <c r="R19" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.15">
@@ -6637,16 +6637,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="92" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C20" s="121" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F20" s="75">
         <v>101</v>
@@ -6664,7 +6664,7 @@
         <v>1</v>
       </c>
       <c r="K20" s="74" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L20" s="74">
         <v>0</v>
@@ -6673,19 +6673,19 @@
         <v>1</v>
       </c>
       <c r="N20" s="85" t="s">
-        <v>111</v>
+        <v>184</v>
       </c>
       <c r="O20" s="99">
-        <v>1.6710292746097057</v>
+        <v>0</v>
       </c>
       <c r="P20" s="83">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="Q20" s="14">
         <v>2</v>
       </c>
       <c r="R20" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="40" customHeight="1" x14ac:dyDescent="0.15">
@@ -6694,16 +6694,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="92" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C21" s="122" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F21" s="75">
         <v>101</v>
@@ -6721,7 +6721,7 @@
         <v>1</v>
       </c>
       <c r="K21" s="74" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L21" s="74">
         <v>0</v>
@@ -6730,13 +6730,13 @@
         <v>1</v>
       </c>
       <c r="N21" s="85" t="s">
-        <v>111</v>
+        <v>184</v>
       </c>
       <c r="O21" s="99">
-        <v>3.3420585492194115</v>
+        <v>0</v>
       </c>
       <c r="P21" s="83">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="Q21" s="14">
         <v>4</v>
@@ -6815,27 +6815,27 @@
         <v>19</v>
       </c>
       <c r="C1" s="95" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D1" s="95" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E1" s="95" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F1" s="95" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="97" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="123" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B2" s="123" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C2" s="124" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D2" s="123"/>
       <c r="E2" s="123"/>
@@ -6843,13 +6843,13 @@
     </row>
     <row r="3" spans="1:6" s="97" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="125" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B3" s="125" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C3" s="126" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D3" s="125"/>
       <c r="E3" s="125"/>
@@ -6857,13 +6857,13 @@
     </row>
     <row r="4" spans="1:6" s="97" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="125" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B4" s="125" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" s="126" t="s">
         <v>178</v>
-      </c>
-      <c r="C4" s="126" t="s">
-        <v>181</v>
       </c>
       <c r="D4" s="125"/>
       <c r="E4" s="125"/>
@@ -6871,13 +6871,13 @@
     </row>
     <row r="5" spans="1:6" s="97" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="127" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B5" s="127" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C5" s="128" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D5" s="127"/>
       <c r="E5" s="127"/>
@@ -6885,13 +6885,13 @@
     </row>
     <row r="6" spans="1:6" s="97" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="125" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B6" s="125" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C6" s="126" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D6" s="125"/>
       <c r="E6" s="125"/>
@@ -6899,13 +6899,13 @@
     </row>
     <row r="7" spans="1:6" s="97" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="125" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B7" s="125" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C7" s="126" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D7" s="125"/>
       <c r="E7" s="125"/>
@@ -6913,13 +6913,13 @@
     </row>
     <row r="8" spans="1:6" s="97" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="125" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B8" s="125" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C8" s="126" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D8" s="125"/>
       <c r="E8" s="125"/>
@@ -6927,13 +6927,13 @@
     </row>
     <row r="9" spans="1:6" s="97" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="125" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B9" s="125" t="s">
+        <v>176</v>
+      </c>
+      <c r="C9" s="126" t="s">
         <v>179</v>
-      </c>
-      <c r="C9" s="126" t="s">
-        <v>182</v>
       </c>
       <c r="D9" s="125"/>
       <c r="E9" s="125"/>
@@ -6941,13 +6941,13 @@
     </row>
     <row r="10" spans="1:6" s="97" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="123" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B10" s="123" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C10" s="124" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D10" s="123"/>
       <c r="E10" s="123"/>
@@ -6955,13 +6955,13 @@
     </row>
     <row r="11" spans="1:6" s="97" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="125" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" s="125" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C11" s="126" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D11" s="125"/>
       <c r="E11" s="125"/>
@@ -6969,13 +6969,13 @@
     </row>
     <row r="12" spans="1:6" s="97" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="125" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" s="125" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C12" s="126" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D12" s="125"/>
       <c r="E12" s="125"/>
@@ -6983,13 +6983,13 @@
     </row>
     <row r="13" spans="1:6" s="97" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="125" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" s="125" t="s">
+        <v>176</v>
+      </c>
+      <c r="C13" s="126" t="s">
         <v>179</v>
-      </c>
-      <c r="C13" s="126" t="s">
-        <v>182</v>
       </c>
       <c r="D13" s="125"/>
       <c r="E13" s="125"/>
@@ -6997,13 +6997,13 @@
     </row>
     <row r="14" spans="1:6" s="97" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="123" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B14" s="123" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C14" s="124" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D14" s="123"/>
       <c r="E14" s="123"/>
@@ -7011,13 +7011,13 @@
     </row>
     <row r="15" spans="1:6" s="97" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="125" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B15" s="125" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C15" s="126" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D15" s="125"/>
       <c r="E15" s="125"/>
@@ -7025,13 +7025,13 @@
     </row>
     <row r="16" spans="1:6" s="97" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="125" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B16" s="125" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C16" s="126" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D16" s="125"/>
       <c r="E16" s="125"/>
@@ -7039,13 +7039,13 @@
     </row>
     <row r="17" spans="1:6" s="97" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="125" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B17" s="125" t="s">
+        <v>176</v>
+      </c>
+      <c r="C17" s="126" t="s">
         <v>179</v>
-      </c>
-      <c r="C17" s="126" t="s">
-        <v>182</v>
       </c>
       <c r="D17" s="125"/>
       <c r="E17" s="125"/>
@@ -7053,13 +7053,13 @@
     </row>
     <row r="18" spans="1:6" s="97" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="123" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B18" s="123" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C18" s="124" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D18" s="123"/>
       <c r="E18" s="123"/>
@@ -7067,13 +7067,13 @@
     </row>
     <row r="19" spans="1:6" s="97" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="125" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B19" s="125" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C19" s="126" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D19" s="125"/>
       <c r="E19" s="125"/>
@@ -7081,13 +7081,13 @@
     </row>
     <row r="20" spans="1:6" s="97" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="125" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B20" s="125" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C20" s="126" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D20" s="125"/>
       <c r="E20" s="125"/>
@@ -7095,13 +7095,13 @@
     </row>
     <row r="21" spans="1:6" s="97" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="125" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B21" s="125" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C21" s="126" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D21" s="125"/>
       <c r="E21" s="125"/>
@@ -7109,13 +7109,13 @@
     </row>
     <row r="22" spans="1:6" s="97" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="123" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B22" s="123" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C22" s="124" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D22" s="123"/>
       <c r="E22" s="123"/>
@@ -7123,13 +7123,13 @@
     </row>
     <row r="23" spans="1:6" s="97" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="125" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B23" s="125" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C23" s="126" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D23" s="125"/>
       <c r="E23" s="125"/>
@@ -7137,13 +7137,13 @@
     </row>
     <row r="24" spans="1:6" s="97" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="125" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B24" s="125" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C24" s="126" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D24" s="125"/>
       <c r="E24" s="125"/>
@@ -7151,13 +7151,13 @@
     </row>
     <row r="25" spans="1:6" s="97" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="127" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B25" s="127" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C25" s="128" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D25" s="127"/>
       <c r="E25" s="127"/>
@@ -7201,90 +7201,90 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="93" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B1" s="93" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C1" s="93" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D1" s="93" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="89" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="89" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B2" s="89" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C2" s="89" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D2" s="89" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="89" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="89" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B3" s="89" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C3" s="89" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D3" s="89" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="89" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="89" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C4" s="89" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="89" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="89" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C5" s="89" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="89" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="89" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="89" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="89" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="89" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="89" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="89" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="89" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="89" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="89" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="89" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="89" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="89" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>